<commit_message>
Crear redes Barabasi-Albert para importar con gephi y analizadas con networkX
</commit_message>
<xml_diff>
--- a/P02/metricas_ba.xlsx
+++ b/P02/metricas_ba.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Teórico" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="GEPHI" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="NetworkX" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="GEPHI" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="39">
   <si>
     <t xml:space="preserve">Scale-free network</t>
   </si>
@@ -84,6 +85,60 @@
   </si>
   <si>
     <t xml:space="preserve">Largest hub Degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.011881094386064566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2304798194957236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0541394705946238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.015794436586515796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.929592173503065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06392553237781687</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.005970137396575216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4712066986292123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.032090817840684176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.007948306277378052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1722610057283305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03668080683651802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0011988011030312268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.034133668479967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.009143936382472708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0015979224612318135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6851372847775727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.010897382950686915</t>
   </si>
 </sst>
 </file>
@@ -304,18 +359,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,6 +817,7 @@
       <c r="I23" s="15"/>
       <c r="J23" s="13"/>
     </row>
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
@@ -784,14 +840,19 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,10 +901,18 @@
       <c r="D3" s="4" t="n">
         <v>1504</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>64</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="n">
@@ -855,12 +924,20 @@
       <c r="D4" s="4" t="n">
         <v>2005</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="n">
         <v>1000</v>
       </c>
@@ -870,12 +947,20 @@
       <c r="D5" s="4" t="n">
         <v>3004</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="n">
         <v>1000</v>
       </c>
@@ -885,12 +970,20 @@
       <c r="D6" s="4" t="n">
         <v>4005</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="n">
         <v>5000</v>
       </c>
@@ -900,12 +993,20 @@
       <c r="D7" s="4" t="n">
         <v>15004</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>221</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="n">
         <v>5000</v>
       </c>
@@ -915,10 +1016,475 @@
       <c r="D8" s="4" t="n">
         <v>20005</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>248</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="14" t="n">
+        <v>500</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A10:H10"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.66"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>1504</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>64</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>3004</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>4005</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>15004</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>221</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>20005</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>248</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>

</xml_diff>

<commit_message>
all Gephi data uploaded
</commit_message>
<xml_diff>
--- a/P02/metricas_ba.xlsx
+++ b/P02/metricas_ba.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hlocal\SOC-master\P02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hlocal\SOC-cebro\P02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Teórico" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="61">
   <si>
     <t>Scale-free network</t>
   </si>
@@ -176,6 +176,39 @@
   </si>
   <si>
     <t>Kmin usado</t>
+  </si>
+  <si>
+    <t>8.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.63</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.94</t>
+  </si>
+  <si>
+    <t>5.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.09</t>
+  </si>
+  <si>
+    <t>3.25</t>
+  </si>
+  <si>
+    <t>4.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.84</t>
+  </si>
+  <si>
+    <t>2.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.97</t>
   </si>
 </sst>
 </file>
@@ -303,15 +336,6 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -365,6 +389,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,643 +693,643 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>500</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>1504</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <f t="shared" ref="E3:E8" si="0">C3/((B3*(B3-1))/2)</f>
         <v>2.4048096192384771E-5</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <f t="shared" ref="F3:F8" si="1">C3*POWER(B3,0.5)</f>
         <v>67.082039324993701</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G8" si="2">LN(B3)/LN(LN(B3))</f>
         <v>3.4017182280363412</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="3">
         <f t="shared" ref="H3:H8" si="3">(LN(B3)*LN(B3))/B3</f>
         <v>7.7242707633949359E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>500</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>2005</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>3.2064128256513025E-5</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <f>C4*POWER(B4,0.5)</f>
         <v>89.442719099991592</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <f t="shared" si="2"/>
         <v>3.4017182280363412</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="3">
         <f t="shared" si="3"/>
         <v>7.7242707633949359E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>1000</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>3004</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>6.006006006006006E-6</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
         <v>94.868329805051374</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <f t="shared" si="2"/>
         <v>3.5742499165819992</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="3">
         <f t="shared" si="3"/>
         <v>4.7717082994305576E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>1000</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>4005</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>8.0080080080080075E-6</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
         <v>126.49110640673517</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <f t="shared" si="2"/>
         <v>3.5742499165819992</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="3">
         <f t="shared" si="3"/>
         <v>4.7717082994305576E-2</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>5000</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>15004</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>2.4004800960192037E-7</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>212.13203435596427</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <f t="shared" si="2"/>
         <v>3.976119453625683</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="3">
         <f t="shared" si="3"/>
         <v>1.4508515971981424E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>5000</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>20005</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>3.2006401280256051E-7</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
         <v>282.84271247461902</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <f t="shared" si="2"/>
         <v>3.976119453625683</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <f t="shared" si="3"/>
         <v>1.4508515971981424E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="K10" s="26"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <v>124.75</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="17">
         <v>0.499</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="17">
         <v>12.454000000000001</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21">
+      <c r="H12" s="17"/>
+      <c r="I12" s="18">
         <v>9.9799999999999997E-4</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="24">
+      <c r="J12" s="19"/>
+      <c r="K12" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="17">
         <v>249.75</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="17">
         <v>0.4995</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="17">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="17">
         <v>13.829000000000001</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21">
+      <c r="H13" s="17"/>
+      <c r="I13" s="18">
         <v>4.9950000000000005E-4</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="24">
+      <c r="J13" s="19"/>
+      <c r="K13" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="17">
         <v>1249.75</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="17">
         <v>0.49990000000000001</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="17">
         <v>1E-4</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="17">
         <v>17.036999999999999</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="21">
+      <c r="H14" s="17"/>
+      <c r="I14" s="18">
         <v>9.9980000000000002E-5</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="24">
+      <c r="J14" s="19"/>
+      <c r="K14" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="17">
         <v>249.5</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="17">
         <v>0.998</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="17">
         <v>2E-3</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="17">
         <v>6.2270000000000003</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21">
+      <c r="H15" s="17"/>
+      <c r="I15" s="18">
         <v>1.9959999999999999E-3</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="25">
+      <c r="J15" s="19"/>
+      <c r="K15" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="17">
         <v>499.5</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="17">
         <v>0.999</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="17">
         <v>6.9139999999999997</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18">
         <v>9.990000000000001E-4</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="25">
+      <c r="J16" s="19"/>
+      <c r="K16" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="17">
         <v>2499.5</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="17">
         <v>0.99980000000000002</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="17">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="17">
         <v>8.5180000000000007</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21">
+      <c r="H17" s="17"/>
+      <c r="I17" s="18">
         <v>1.9996E-4</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="25">
+      <c r="J17" s="19"/>
+      <c r="K17" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="17">
         <v>898.2</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="17">
         <v>3.5928</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="17">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="17">
         <v>1.73</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="17">
         <v>4.859</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="18">
         <v>7.1856000000000003E-3</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="25">
+      <c r="J18" s="19"/>
+      <c r="K18" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="17">
         <v>1973.0250000000001</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="17">
         <v>3.9460500000000001</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="17">
         <v>3.9500000000000004E-3</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="17">
         <v>1.75</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="17">
         <v>5.032</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="18">
         <v>3.9460500000000004E-3</v>
       </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="25">
+      <c r="J19" s="19"/>
+      <c r="K19" s="22">
         <v>0</v>
       </c>
-      <c r="M19" s="26"/>
+      <c r="M19" s="23"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="17">
         <v>11872.625</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="17">
         <v>4.7490500000000004</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="17">
         <v>9.5E-4</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="17">
         <v>1.7929999999999999</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="17">
         <v>5.4589999999999996</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="18">
         <v>9.5980999999999996E-4</v>
       </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="25">
+      <c r="J20" s="19"/>
+      <c r="K20" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="17">
         <v>500</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="17">
         <v>2495</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="17">
         <v>9.98</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="17">
         <v>0.02</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="17">
         <v>2.6219999999999999</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="17">
         <v>2.7010000000000001</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="18">
         <v>1.9959999999999999E-2</v>
       </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="25">
+      <c r="J21" s="19"/>
+      <c r="K21" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="17">
         <v>4995</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="17">
         <v>9.99</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="17">
         <v>0.01</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="17">
         <v>2.6909999999999998</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="17">
         <v>3.0009999999999999</v>
       </c>
-      <c r="I22" s="21">
+      <c r="I22" s="18">
         <v>9.9900000000000006E-3</v>
       </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="25">
+      <c r="J22" s="19"/>
+      <c r="K22" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <v>24995</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="17">
         <v>9.9979999999999993</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="17">
         <v>2E-3</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="17">
         <v>2.851</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="17">
         <v>3.6989999999999998</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="18">
         <v>1.9995999999999998E-3</v>
       </c>
-      <c r="J23" s="22"/>
-      <c r="K23" s="25">
+      <c r="J23" s="19"/>
+      <c r="K23" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1315,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="B12:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1331,520 +1364,520 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>500</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>1504</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>64</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>500</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>2005</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>83</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>1000</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>3004</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <v>100</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>1000</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>4005</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>111</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>5000</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>15004</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>221</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>5000</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>20005</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <v>248</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <v>105</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="17">
         <v>0.42399999999999999</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="22"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="17">
         <v>231</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="17">
         <v>0.46400000000000002</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="17">
         <v>0</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="22"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="17">
         <v>1249</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="17">
         <v>0.5</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="17">
         <v>0</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="22"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="17">
         <v>262</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="17">
         <v>1.052</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="17">
         <v>2E-3</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="22"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="17">
         <v>502</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="17">
         <v>1.006</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="22"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="17">
         <v>2514</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="17">
         <v>1.006</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="17">
         <v>0</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="22"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="17">
         <v>904</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="17">
         <v>3.62</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="17">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="22"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="17">
         <v>1874</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="17">
         <v>3.75</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="17">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="22"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="17">
         <v>11816</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="17">
         <v>4.7270000000000003</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="22"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="19"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="17">
         <v>500</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="17">
         <v>2416</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="17">
         <v>9.8480000000000008</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="17">
         <v>0.02</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="22"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="17">
         <v>5019</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="17">
         <v>10.039999999999999</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="17">
         <v>0.01</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="22"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <v>25092</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="17">
         <v>10.37</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="17">
         <v>2E-3</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="22"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1860,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1876,424 +1909,616 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>500</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>1504</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>64</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>500</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>2005</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>83</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>1000</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>3004</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <v>100</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>1000</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>4005</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>111</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>5000</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>15004</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>221</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>5000</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>20005</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <v>248</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="14"/>
+      <c r="C12" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="17">
+        <v>105</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="G12" s="12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>394</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="14"/>
+      <c r="C13" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="17">
+        <v>231</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>5</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>768</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="14"/>
+      <c r="C14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1249</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>4</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>3750</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="14"/>
+      <c r="C15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="17">
+        <v>262</v>
+      </c>
+      <c r="E15" s="17">
+        <v>1.052</v>
+      </c>
+      <c r="F15" s="17">
+        <v>2E-3</v>
+      </c>
+      <c r="G15" s="12">
+        <v>4</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J15" s="11">
+        <v>238</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14"/>
+      <c r="C16" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="17">
+        <v>502</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1.006</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="G16" s="12">
+        <v>6</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>498</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="14"/>
+      <c r="C17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="17">
+        <v>2514</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1.006</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>7</v>
+      </c>
+      <c r="H17" s="13">
+        <v>18924</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>2486</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="14"/>
+      <c r="C18" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="17">
+        <v>904</v>
+      </c>
+      <c r="E18" s="17">
+        <v>3.62</v>
+      </c>
+      <c r="F18" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G18" s="12">
+        <v>9</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J18" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="14"/>
+      <c r="C19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1874</v>
+      </c>
+      <c r="E19" s="17">
+        <v>3.75</v>
+      </c>
+      <c r="F19" s="17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G19" s="12">
+        <v>12</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J19" s="11">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="14"/>
+      <c r="C20" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="17">
+        <v>11816</v>
+      </c>
+      <c r="E20" s="17">
+        <v>4.7270000000000003</v>
+      </c>
+      <c r="F20" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="G20" s="12">
+        <v>15</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="J20" s="11">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="17">
         <v>500</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="14"/>
+      <c r="C21" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="17">
+        <v>2416</v>
+      </c>
+      <c r="E21" s="17">
+        <v>9.8480000000000008</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.02</v>
+      </c>
+      <c r="G21" s="12">
+        <v>21</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="14"/>
+      <c r="C22" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="17">
+        <v>5019</v>
+      </c>
+      <c r="E22" s="17">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="G22" s="12">
+        <v>20</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="14"/>
+      <c r="C23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="17">
+        <v>25092</v>
+      </c>
+      <c r="E23" s="17">
+        <v>10.37</v>
+      </c>
+      <c r="F23" s="17">
+        <v>2E-3</v>
+      </c>
+      <c r="G23" s="12">
+        <v>24</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="12">
+        <v>2E-3</v>
+      </c>
+      <c r="J23" s="11">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2301,6 +2526,6 @@
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>